<commit_message>
Resolved the issues rlated to verify hyper links
</commit_message>
<xml_diff>
--- a/AutoRepository/database/HeaderLinks.xlsx
+++ b/AutoRepository/database/HeaderLinks.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Header" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Header1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Header2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
   <si>
     <t xml:space="preserve">Links To be Clicked</t>
   </si>
@@ -31,6 +32,39 @@
     <t xml:space="preserve">Name of Link</t>
   </si>
   <si>
+    <t xml:space="preserve">Dwarf Rabbit Disaster Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piggy Rescue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bunny Buddies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pot-bellied Pals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flop-ear Families</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animal Action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give to any Canadian charity | CHIMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Athiest Alms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food Banks of BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clean Water for all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Justice for the poor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Account Settings</t>
   </si>
   <si>
@@ -41,39 +75,6 @@
   </si>
   <si>
     <t xml:space="preserve">Giving Tools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dwarf Rabbit Disaster Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Piggy Rescue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bunny Buddies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pot-bellied Pals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flop-ear Families</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Animal Action</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Give to any Canadian charity | CHIMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Athiest Alms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Food Banks of BC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clean Water for all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justice for the poor</t>
   </si>
 </sst>
 </file>
@@ -185,18 +186,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -215,86 +216,86 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="C8" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="0" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>11</v>
       </c>
     </row>
@@ -303,7 +304,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>12</v>
@@ -311,46 +312,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -362,4 +330,78 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>